<commit_message>
XGBoost on noisy data completed and all algos on filtered data completed. Summary sheet updated for both smooth and noisy data
</commit_message>
<xml_diff>
--- a/Capstone_Two/Modelling/Modelling Summary.xlsx
+++ b/Capstone_Two/Modelling/Modelling Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Springboard\Technical Project\7_Capstone Two\7_Modelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1581EF62-774A-42ED-B0DA-33642E96B2E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19E5078-CEA9-492D-86ED-7B5642ECCCAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="18">
   <si>
     <t>S. No.</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Noisy Data</t>
+  </si>
+  <si>
+    <t>Clean Data</t>
   </si>
 </sst>
 </file>
@@ -151,7 +154,91 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -484,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:AG8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,9 +583,12 @@
     <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="16" width="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="33" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -517,8 +607,26 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
+      <c r="R1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
     </row>
-    <row r="2" spans="1:16" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,8 +661,42 @@
         <v>9</v>
       </c>
       <c r="P2" s="3"/>
+      <c r="R2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG2" s="3"/>
     </row>
-    <row r="3" spans="1:16" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="86.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
@@ -599,8 +741,52 @@
       <c r="P3" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -649,8 +835,56 @@
       <c r="P4" s="4">
         <v>71.53</v>
       </c>
+      <c r="R4" s="1">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T4" s="4">
+        <v>93.05</v>
+      </c>
+      <c r="U4" s="4">
+        <v>77.540000000000006</v>
+      </c>
+      <c r="V4" s="4">
+        <v>91.47</v>
+      </c>
+      <c r="W4" s="4">
+        <v>71.64</v>
+      </c>
+      <c r="X4" s="4">
+        <v>46.84</v>
+      </c>
+      <c r="Y4" s="4">
+        <v>17.54</v>
+      </c>
+      <c r="Z4" s="4">
+        <v>93.83</v>
+      </c>
+      <c r="AA4" s="4">
+        <v>78.77</v>
+      </c>
+      <c r="AB4" s="4">
+        <v>93.72</v>
+      </c>
+      <c r="AC4" s="4">
+        <v>77.540000000000006</v>
+      </c>
+      <c r="AD4" s="4">
+        <v>91.69</v>
+      </c>
+      <c r="AE4" s="4">
+        <v>70.260000000000005</v>
+      </c>
+      <c r="AF4" s="4">
+        <v>94.02</v>
+      </c>
+      <c r="AG4" s="4">
+        <v>79.08</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -699,8 +933,56 @@
       <c r="P5" s="4">
         <v>74.06</v>
       </c>
+      <c r="R5" s="1">
+        <v>2</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T5" s="4">
+        <v>98.7</v>
+      </c>
+      <c r="U5" s="4">
+        <v>86.28</v>
+      </c>
+      <c r="V5" s="4">
+        <v>98.3</v>
+      </c>
+      <c r="W5" s="4">
+        <v>83.75</v>
+      </c>
+      <c r="X5" s="4">
+        <v>52.65</v>
+      </c>
+      <c r="Y5" s="4">
+        <v>16.93</v>
+      </c>
+      <c r="Z5" s="4">
+        <v>98.86</v>
+      </c>
+      <c r="AA5" s="4">
+        <v>88.35</v>
+      </c>
+      <c r="AB5" s="4">
+        <v>98.73</v>
+      </c>
+      <c r="AC5" s="4">
+        <v>85.59</v>
+      </c>
+      <c r="AD5" s="4">
+        <v>98.3</v>
+      </c>
+      <c r="AE5" s="4">
+        <v>85.05</v>
+      </c>
+      <c r="AF5" s="4">
+        <v>98.81</v>
+      </c>
+      <c r="AG5" s="4">
+        <v>87.89</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -749,8 +1031,56 @@
       <c r="P6" s="4">
         <v>85.46</v>
       </c>
+      <c r="R6" s="1">
+        <v>3</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T6" s="4">
+        <v>98.73</v>
+      </c>
+      <c r="U6" s="4">
+        <v>89.42</v>
+      </c>
+      <c r="V6" s="4">
+        <v>98.87</v>
+      </c>
+      <c r="W6" s="4">
+        <v>88.5</v>
+      </c>
+      <c r="X6" s="4">
+        <v>29.68</v>
+      </c>
+      <c r="Y6" s="4">
+        <v>10.26</v>
+      </c>
+      <c r="Z6" s="4">
+        <v>99.09</v>
+      </c>
+      <c r="AA6" s="4">
+        <v>90.72</v>
+      </c>
+      <c r="AB6" s="4">
+        <v>98.74</v>
+      </c>
+      <c r="AC6" s="4">
+        <v>89.57</v>
+      </c>
+      <c r="AD6" s="4">
+        <v>98.95</v>
+      </c>
+      <c r="AE6" s="4">
+        <v>88.88</v>
+      </c>
+      <c r="AF6" s="4">
+        <v>99.24</v>
+      </c>
+      <c r="AG6" s="4">
+        <v>90.65</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -799,32 +1129,164 @@
       <c r="P7" s="4">
         <v>87.98</v>
       </c>
+      <c r="R7" s="1">
+        <v>4</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T7" s="4">
+        <v>98.96</v>
+      </c>
+      <c r="U7" s="4">
+        <v>89.5</v>
+      </c>
+      <c r="V7" s="4">
+        <v>98.73</v>
+      </c>
+      <c r="W7" s="4">
+        <v>89.96</v>
+      </c>
+      <c r="X7" s="4">
+        <v>50.88</v>
+      </c>
+      <c r="Y7" s="4">
+        <v>17.47</v>
+      </c>
+      <c r="Z7" s="4">
+        <v>99</v>
+      </c>
+      <c r="AA7" s="4">
+        <v>90.88</v>
+      </c>
+      <c r="AB7" s="4">
+        <v>98.77</v>
+      </c>
+      <c r="AC7" s="4">
+        <v>90.26</v>
+      </c>
+      <c r="AD7" s="4">
+        <v>98.82</v>
+      </c>
+      <c r="AE7" s="4">
+        <v>89.88</v>
+      </c>
+      <c r="AF7" s="4">
+        <v>99.13</v>
+      </c>
+      <c r="AG7" s="4">
+        <v>91.34</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
+      <c r="C8" s="4">
+        <v>97.63</v>
+      </c>
+      <c r="D8" s="4">
+        <v>82.78</v>
+      </c>
+      <c r="E8" s="4">
+        <v>97.53</v>
+      </c>
+      <c r="F8" s="4">
+        <v>82.17</v>
+      </c>
+      <c r="G8" s="4">
+        <v>43.55</v>
+      </c>
+      <c r="H8" s="4">
+        <v>14.92</v>
+      </c>
+      <c r="I8" s="4">
+        <v>98.21</v>
+      </c>
+      <c r="J8" s="4">
+        <v>86.38</v>
+      </c>
+      <c r="K8" s="4">
+        <v>97.44</v>
+      </c>
+      <c r="L8" s="4">
+        <v>83.39</v>
+      </c>
+      <c r="M8" s="4">
+        <v>97.75</v>
+      </c>
+      <c r="N8" s="4">
+        <v>82.47</v>
+      </c>
+      <c r="O8" s="4">
+        <v>98.33</v>
+      </c>
+      <c r="P8" s="4">
+        <v>85.69</v>
+      </c>
+      <c r="R8" s="1">
+        <v>5</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T8" s="4">
+        <v>98.25</v>
+      </c>
+      <c r="U8" s="4">
+        <v>88.42</v>
+      </c>
+      <c r="V8" s="4">
+        <v>98.1</v>
+      </c>
+      <c r="W8" s="4">
+        <v>87.04</v>
+      </c>
+      <c r="X8" s="4">
+        <v>47.09</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>16.16</v>
+      </c>
+      <c r="Z8" s="4">
+        <v>98.59</v>
+      </c>
+      <c r="AA8" s="4">
+        <v>90.11</v>
+      </c>
+      <c r="AB8" s="4">
+        <v>98.29</v>
+      </c>
+      <c r="AC8" s="4">
+        <v>88.04</v>
+      </c>
+      <c r="AD8" s="4">
+        <v>98.2</v>
+      </c>
+      <c r="AE8" s="4">
+        <v>87.12</v>
+      </c>
+      <c r="AF8" s="4">
+        <v>98.59</v>
+      </c>
+      <c r="AG8" s="4">
+        <v>89.96</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="16">
     <mergeCell ref="A1:P1"/>
+    <mergeCell ref="R1:AG1"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
@@ -834,27 +1296,63 @@
     <mergeCell ref="M2:N2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4 E4 G4 I4 K4 M4 O4">
+    <cfRule type="top10" dxfId="19" priority="20" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4 F4 H4 J4 L4 N4 P4">
+    <cfRule type="top10" dxfId="18" priority="19" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5 E5 G5 I5 K5 M5 O5">
+    <cfRule type="top10" dxfId="17" priority="18" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5 F5 H5 J5 L5 N5 P5">
+    <cfRule type="top10" dxfId="16" priority="17" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6 E6 G6 I6 K6 M6 O6">
+    <cfRule type="top10" dxfId="15" priority="16" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6 F6 H6 J6 L6 N6 P6">
+    <cfRule type="top10" dxfId="14" priority="15" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7 E7 G7 I7 K7 M7 O7">
+    <cfRule type="top10" dxfId="13" priority="14" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7 F7 H7 J7 L7 N7 P7">
+    <cfRule type="top10" dxfId="12" priority="13" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8 E8 G8 I8 K8 M8 O8">
+    <cfRule type="top10" dxfId="11" priority="12" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8 F8 H8 J8 L8 N8 P8">
+    <cfRule type="top10" dxfId="10" priority="11" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T4 V4 X4 Z4 AB4 AD4 AF4">
+    <cfRule type="top10" dxfId="9" priority="10" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U4 W4 Y4 AA4 AC4 AE4 AG4">
+    <cfRule type="top10" dxfId="8" priority="9" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T5 V5 X5 Z5 AB5 AD5 AF5">
     <cfRule type="top10" dxfId="7" priority="8" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4 F4 H4 J4 L4 N4 P4">
+  <conditionalFormatting sqref="U5 W5 Y5 AA5 AC5 AE5 AG5">
     <cfRule type="top10" dxfId="6" priority="7" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5 E5 G5 I5 K5 M5 O5">
+  <conditionalFormatting sqref="T6 V6 X6 Z6 AB6 AD6 AF6">
     <cfRule type="top10" dxfId="5" priority="6" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5 F5 H5 J5 L5 N5 P5">
+  <conditionalFormatting sqref="U6 W6 Y6 AA6 AC6 AE6 AG6">
     <cfRule type="top10" dxfId="4" priority="5" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6 E6 G6 I6 K6 M6 O6">
+  <conditionalFormatting sqref="T7 V7 X7 Z7 AB7 AD7 AF7">
     <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6 F6 H6 J6 L6 N6 P6">
+  <conditionalFormatting sqref="U7 W7 Y7 AA7 AC7 AE7 AG7">
     <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7 E7 G7 I7 K7 M7 O7">
+  <conditionalFormatting sqref="T8 V8 X8 Z8 AB8 AD8 AF8">
     <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D7 F7 H7 J7 L7 N7 P7">
+  <conditionalFormatting sqref="U8 W8 Y8 AA8 AC8 AE8 AG8">
     <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>